<commit_message>
Fixed part numbering (duplicate R5)
</commit_message>
<xml_diff>
--- a/Sprite_Files/SpriteBOM.xlsx
+++ b/Sprite_Files/SpriteBOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="620" windowWidth="27560" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="1240" yWindow="620" windowWidth="27560" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -254,9 +254,6 @@
     <t>P1, P2</t>
   </si>
   <si>
-    <t>R3, R4, R5, R7</t>
-  </si>
-  <si>
     <t>S1, S2, S3, S4</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>OSC TCXO 26.000MHZ CLPD SNWV SMD</t>
+  </si>
+  <si>
+    <t>R3, R4, R6, R7</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>42</v>
@@ -728,7 +728,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>43</v>
@@ -751,7 +751,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>44</v>
@@ -774,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>45</v>
@@ -797,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>47</v>
@@ -820,7 +820,7 @@
         <v>57</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>48</v>
@@ -843,7 +843,7 @@
         <v>49</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>46</v>
@@ -866,7 +866,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>50</v>
@@ -889,7 +889,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>51</v>
@@ -912,7 +912,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>52</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
@@ -935,7 +935,7 @@
         <v>61</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>60</v>
@@ -958,7 +958,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>53</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
@@ -981,7 +981,7 @@
         <v>28</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>41</v>
@@ -1004,7 +1004,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>40</v>
@@ -1027,7 +1027,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>55</v>
@@ -1050,7 +1050,7 @@
         <v>38</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>54</v>

</xml_diff>